<commit_message>
T1: Final To Print file; T2: DPU proper with good scenario, to little refactor
</commit_message>
<xml_diff>
--- a/Fizyka_Sprawka/EndTableKulka.xlsx
+++ b/Fizyka_Sprawka/EndTableKulka.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>L.p.</t>
   </si>
@@ -88,12 +88,51 @@
       <t>π</t>
     </r>
   </si>
+  <si>
+    <t>Tulejka</t>
+  </si>
+  <si>
+    <t>h[mm]</t>
+  </si>
+  <si>
+    <t>dwew[mm]</t>
+  </si>
+  <si>
+    <t>dzew[mm]</t>
+  </si>
+  <si>
+    <t>2.3π</t>
+  </si>
+  <si>
+    <t>360π</t>
+  </si>
+  <si>
+    <t>90.789666π</t>
+  </si>
+  <si>
+    <t>0.018170375π</t>
+  </si>
+  <si>
+    <r>
+      <t>0.014426063 1/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>π</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +147,21 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -275,27 +329,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -303,19 +454,68 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -340,9 +540,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>21535</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="329453" cy="138952"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -354,7 +554,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="447675" y="2333625"/>
+              <a:off x="0" y="2612335"/>
               <a:ext cx="329453" cy="138952"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -435,7 +635,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="447675" y="2333625"/>
+              <a:off x="0" y="2612335"/>
               <a:ext cx="329453" cy="138952"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -499,9 +699,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>23605</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>7040</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="381323" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -513,7 +713,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="276225" y="2486025"/>
+              <a:off x="23605" y="2797865"/>
               <a:ext cx="381323" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -541,6 +741,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -555,7 +756,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -568,7 +769,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -582,7 +783,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -598,7 +799,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -611,7 +812,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -635,7 +836,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="276225" y="2486025"/>
+              <a:off x="23605" y="2797865"/>
               <a:ext cx="381323" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -663,13 +864,14 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -686,9 +888,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>15323</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>196298</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="387670" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -700,7 +902,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="266700" y="2667000"/>
+              <a:off x="15323" y="2987123"/>
               <a:ext cx="387670" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -728,6 +930,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -742,7 +945,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -755,7 +958,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -785,7 +988,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -798,7 +1001,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -822,7 +1025,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="266700" y="2667000"/>
+              <a:off x="15323" y="2987123"/>
               <a:ext cx="387670" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -850,13 +1053,14 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -880,7 +1084,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -897,9 +1101,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>41413</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>189257</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="381323" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -911,7 +1115,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="247650" y="2876550"/>
+              <a:off x="41413" y="3180107"/>
               <a:ext cx="381323" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -939,6 +1143,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -953,7 +1158,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -966,7 +1171,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -996,7 +1201,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1009,7 +1214,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -1033,7 +1238,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="247650" y="2876550"/>
+              <a:off x="41413" y="3180107"/>
               <a:ext cx="381323" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1061,13 +1266,14 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1091,7 +1297,781 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> (𝑥)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12010</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="329453" cy="138952"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="6193735"/>
+              <a:ext cx="329453" cy="138952"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̅"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                    <m:r>
+                      <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="6193735"/>
+              <a:ext cx="329453" cy="138952"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> ̅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>  </a:t>
+              </a:r>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="pl-PL" sz="1100" b="0"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>33130</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>197540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="381323" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="33130" y="6379265"/>
+              <a:ext cx="381323" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑢</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐴</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="33130" y="6379265"/>
+              <a:ext cx="381323" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑢_𝐴 (𝑥)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>24848</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>5798</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="387670" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="24848" y="6587573"/>
+              <a:ext cx="387670" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑢</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐵</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="24848" y="6587573"/>
+              <a:ext cx="387670" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑢_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐵</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> (𝑥)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>31888</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>198782</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="381323" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="TextBox 12"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="31888" y="6780557"/>
+              <a:ext cx="381323" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑢</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐶</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="TextBox 12"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="31888" y="6780557"/>
+              <a:ext cx="381323" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑢_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐶</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1371,213 +2351,517 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="2">
         <v>8.44</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B5" s="3">
         <v>8.44</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B6" s="4">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B7" s="4">
         <v>8.17</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B8" s="5">
         <v>8.01</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B9" s="5">
         <v>8.06</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B10" s="5">
         <v>8.02</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B11" s="5">
         <v>8.02</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B12" s="5">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B13" s="4">
         <v>8.41</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="7">
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4">
         <v>8.1669999999999998</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C14" s="6">
         <v>0.72</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E14" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="7">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4">
         <v>0.06</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="7">
         <v>0</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="7">
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C16" s="7">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="15">
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C17" s="10">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D16" s="16">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="D17" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="30"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2">
+        <v>34.15</v>
+      </c>
+      <c r="C21" s="24">
+        <v>12</v>
+      </c>
+      <c r="D21" s="24">
+        <v>15.18</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3">
+        <v>34</v>
+      </c>
+      <c r="C22" s="25">
+        <v>11.95</v>
+      </c>
+      <c r="D22" s="7">
+        <v>15.75</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5">
+        <v>34.1</v>
+      </c>
+      <c r="C23" s="6">
+        <v>12</v>
+      </c>
+      <c r="D23" s="7">
+        <v>15.8</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
+      <c r="B24" s="5">
+        <v>34.1</v>
+      </c>
+      <c r="C24" s="25">
+        <v>12</v>
+      </c>
+      <c r="D24" s="7">
+        <v>15.85</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5">
+        <v>34.1</v>
+      </c>
+      <c r="C25" s="25">
+        <v>12</v>
+      </c>
+      <c r="D25" s="7">
+        <v>15.8</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="C26" s="25">
+        <v>12.75</v>
+      </c>
+      <c r="D26" s="7">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="B27" s="5">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="C27" s="25">
+        <v>12.9</v>
+      </c>
+      <c r="D27" s="7">
+        <v>16</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>8</v>
+      </c>
+      <c r="B28" s="5">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="C28" s="25">
+        <v>11.8</v>
+      </c>
+      <c r="D28" s="7">
+        <v>16</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5">
+        <v>34.4</v>
+      </c>
+      <c r="C29" s="25">
+        <v>11.8</v>
+      </c>
+      <c r="D29" s="7">
+        <v>16</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4">
+        <v>34</v>
+      </c>
+      <c r="C30" s="7">
+        <v>12.95</v>
+      </c>
+      <c r="D30" s="7">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="4">
+        <f>AVERAGE(B21:B30)</f>
+        <v>34.169999999999995</v>
+      </c>
+      <c r="C31" s="7">
+        <f>AVERAGE(C21:C30)</f>
+        <v>12.215</v>
+      </c>
+      <c r="D31" s="7">
+        <f>AVERAGE(D21:D30)</f>
+        <v>15.858000000000001</v>
+      </c>
+      <c r="E31" s="6">
+        <v>8.24</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="26">
+        <v>0.06</v>
+      </c>
+      <c r="C32" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="D32" s="25">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E32" s="25">
+        <v>0</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="26">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C33" s="25">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D33" s="25">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E33" s="25">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="31">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C34" s="32">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="D34" s="32">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="E34" s="32">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E12"/>
+  <mergeCells count="6">
+    <mergeCell ref="F32:G33"/>
+    <mergeCell ref="C4:E13"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="A18:G19"/>
+    <mergeCell ref="E21:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>